<commit_message>
Added Better package folder
</commit_message>
<xml_diff>
--- a/ME342NumAnalysis/Other/HandIteration.xlsx
+++ b/ME342NumAnalysis/Other/HandIteration.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\Engineering\ME342NumAnalysis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\Engineering\ME342NumAnalysis\Other\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCEE8AB5-8A1E-4E8E-A081-534B701AAE65}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC3F133C-7B4B-4AE6-BF9C-C535027F1C7B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{8AAD77C3-8360-42E0-8AA8-B9230A28FA7A}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{8AAD77C3-8360-42E0-8AA8-B9230A28FA7A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="100">
   <si>
     <t xml:space="preserve">Iteration </t>
   </si>
@@ -291,6 +291,48 @@
   </si>
   <si>
     <t>Step Size</t>
+  </si>
+  <si>
+    <t>dx/dt</t>
+  </si>
+  <si>
+    <t>Embedded Runge-Kutta</t>
+  </si>
+  <si>
+    <t>k6</t>
+  </si>
+  <si>
+    <t>k5</t>
+  </si>
+  <si>
+    <t>y4</t>
+  </si>
+  <si>
+    <t>y5</t>
+  </si>
+  <si>
+    <t>stepsize:</t>
+  </si>
+  <si>
+    <t>Error est</t>
+  </si>
+  <si>
+    <t>yscale</t>
+  </si>
+  <si>
+    <t>error tol</t>
+  </si>
+  <si>
+    <t>desired err</t>
+  </si>
+  <si>
+    <t>alpha</t>
+  </si>
+  <si>
+    <t>hNew</t>
+  </si>
+  <si>
+    <t>FS</t>
   </si>
 </sst>
 </file>
@@ -608,7 +650,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -640,6 +682,8 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2988,10 +3032,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEB9CBC2-794F-4C8C-B65A-6B36D65342DB}">
-  <dimension ref="A1:Q102"/>
+  <dimension ref="A1:Q124"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" zoomScale="143" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="C88" sqref="C88"/>
+    <sheetView tabSelected="1" topLeftCell="A81" zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
+      <selection activeCell="F115" sqref="F115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4909,24 +4953,24 @@
         <v>1</v>
       </c>
       <c r="G81" s="1">
-        <f>($E81)*SIN($F81)^3</f>
+        <f>($F81)*SIN($E81)^3</f>
         <v>0</v>
       </c>
       <c r="H81" s="1">
-        <f>($E81+0.5*$H$79)*SIN($F81+0.5*G81*$H$79)^3</f>
-        <v>0.2979116182954778</v>
+        <f>($F81+0.5*G81*$H$79)*SIN($E81+0.5*$H$79)^3</f>
+        <v>0.11019540730213864</v>
       </c>
       <c r="I81" s="1">
-        <f>($E81+0.5*$H$79)*SIN($F81+0.5*H81*$H$79)^3</f>
-        <v>0.37969574596407357</v>
+        <f>($F81+0.5*H81*$H$79)*SIN($E81+0.5*$H$79)^3</f>
+        <v>0.11626692119738076</v>
       </c>
       <c r="J81" s="1">
-        <f>($E81+$H$79)*SIN($F81+I81*$H$79)^3</f>
-        <v>0.94637550529092329</v>
+        <f>($F81+I81*$H$79)*SIN($E81+$H$79)^3</f>
+        <v>0.66509776988724456</v>
       </c>
       <c r="K81" s="22">
         <f>1/6*(G81+2*H81+2*I81+J81)*$H$79</f>
-        <v>0.38359837230167099</v>
+        <v>0.18633707114771392</v>
       </c>
     </row>
     <row r="82" spans="1:11" x14ac:dyDescent="0.3">
@@ -4946,27 +4990,27 @@
       </c>
       <c r="F82" s="1">
         <f>F81+K81</f>
-        <v>1.3835983723016709</v>
+        <v>1.1863370711477139</v>
       </c>
       <c r="G82" s="1">
-        <f t="shared" ref="G82:G84" si="45">($E82)*SIN($F82)^3</f>
-        <v>0.94849902714842693</v>
+        <f t="shared" ref="G82:G84" si="45">($F82)*SIN($E82)^3</f>
+        <v>0.70684719341906566</v>
       </c>
       <c r="H82" s="1">
-        <f t="shared" ref="H82:I82" si="46">($E82+0.5*$H$79)*SIN($F82+0.5*G82*$H$79)^3</f>
-        <v>1.3233039138770519</v>
+        <f t="shared" ref="H82:I82" si="46">($F82+0.5*G82*$H$79)*SIN($E82+0.5*$H$79)^3</f>
+        <v>1.5282182667749313</v>
       </c>
       <c r="I82" s="1">
         <f t="shared" si="46"/>
-        <v>1.0558228713289766</v>
+        <v>1.9358252099532398</v>
       </c>
       <c r="J82" s="1">
-        <f t="shared" ref="J82:J84" si="47">($E82+$H$79)*SIN($F82+I82*$H$79)^3</f>
-        <v>0.53886423410484863</v>
+        <f t="shared" ref="J82:J84" si="47">($F82+I82*$H$79)*SIN($E82+$H$79)^3</f>
+        <v>2.3473257285609028</v>
       </c>
       <c r="K82" s="22">
         <f t="shared" ref="K82:K84" si="48">1/6*(G82+2*H82+2*I82+J82)*$H$79</f>
-        <v>1.0409361386108889</v>
+        <v>1.6637099792393848</v>
       </c>
     </row>
     <row r="83" spans="1:11" x14ac:dyDescent="0.3">
@@ -4986,27 +5030,27 @@
       </c>
       <c r="F83" s="1">
         <f>F82+K82</f>
-        <v>2.4245345109125598</v>
+        <v>2.8500470503870989</v>
       </c>
       <c r="G83" s="1">
         <f t="shared" si="45"/>
-        <v>0.56762748416502584</v>
+        <v>2.1427421660554078</v>
       </c>
       <c r="H83" s="1">
-        <f t="shared" ref="H83:I83" si="50">($E83+0.5*$H$79)*SIN($F83+0.5*G83*$H$79)^3</f>
-        <v>0.18497885866064143</v>
+        <f t="shared" ref="H83:I83" si="50">($F83+0.5*G83*$H$79)*SIN($E83+0.5*$H$79)^3</f>
+        <v>0.84057210915788816</v>
       </c>
       <c r="I83" s="1">
         <f t="shared" si="50"/>
-        <v>0.49985615349309642</v>
+        <v>0.70100935482143112</v>
       </c>
       <c r="J83" s="1">
         <f t="shared" si="47"/>
-        <v>3.0022869625584786E-2</v>
+        <v>9.9798347124089807E-3</v>
       </c>
       <c r="K83" s="22">
         <f t="shared" si="48"/>
-        <v>0.32788672968301436</v>
+        <v>0.87264748812107584</v>
       </c>
     </row>
     <row r="84" spans="1:11" x14ac:dyDescent="0.3">
@@ -5026,27 +5070,27 @@
       </c>
       <c r="F84" s="1">
         <f>F83+K83</f>
-        <v>2.7524212405955741</v>
+        <v>3.7226945385081747</v>
       </c>
       <c r="G84" s="1">
         <f t="shared" si="45"/>
-        <v>0.16386586574229661</v>
+        <v>1.0462203902085731E-2</v>
       </c>
       <c r="H84" s="1">
-        <f t="shared" ref="H84:I84" si="51">($E84+0.5*$H$79)*SIN($F84+0.5*G84*$H$79)^3</f>
-        <v>9.6812684756003298E-2</v>
+        <f t="shared" ref="H84:I84" si="51">($F84+0.5*G84*$H$79)*SIN($E84+0.5*$H$79)^3</f>
+        <v>-0.16091024670997162</v>
       </c>
       <c r="I84" s="1">
         <f t="shared" si="51"/>
-        <v>0.13065306879783442</v>
+        <v>-0.15721173097135271</v>
       </c>
       <c r="J84" s="1">
         <f t="shared" si="47"/>
-        <v>6.6832744229562729E-2</v>
+        <v>-1.5454893357609343</v>
       </c>
       <c r="K84" s="22">
         <f t="shared" si="48"/>
-        <v>0.11427168617992246</v>
+        <v>-0.36187851453691616</v>
       </c>
     </row>
     <row r="85" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -5063,7 +5107,7 @@
       </c>
       <c r="F85" s="26">
         <f>ABS(F84-B91)/B91</f>
-        <v>0.27439721490796498</v>
+        <v>1.8610420037323439E-2</v>
       </c>
       <c r="G85" s="24"/>
       <c r="H85" s="24"/>
@@ -5142,24 +5186,24 @@
         <v>1</v>
       </c>
       <c r="G89" s="1">
-        <f>($E89)*SIN($F89)^3</f>
+        <f>($F89)*SIN($E89)^3</f>
         <v>0</v>
       </c>
       <c r="H89" s="1">
-        <f>($E89+0.5*$H$87)*SIN($F89+0.5*G89*$H$87)^3</f>
-        <v>0.1489558091477389</v>
+        <f>($F89+0.5*G89*$H$87)*SIN($E89+0.5*$H$87)^3</f>
+        <v>1.5143279435058658E-2</v>
       </c>
       <c r="I89" s="1">
-        <f>($E89+0.5*$H$87)*SIN($F89+0.5*H89*$H$87)^3</f>
-        <v>0.15957114862293986</v>
+        <f>($F89+0.5*H89*$H$87)*SIN($E89+0.5*$H$87)^3</f>
+        <v>1.5200609163070724E-2</v>
       </c>
       <c r="J89" s="1">
-        <f>($E89+$H$87)*SIN($F89+I89*$H$87)^3</f>
-        <v>0.34289732171700671</v>
+        <f>($F89+I89*$H$87)*SIN($E89+$H$87)^3</f>
+        <v>0.11103292596112124</v>
       </c>
       <c r="K89" s="22">
-        <f>1/6*(G89+2*H89+2*I89+J89)*$H$87</f>
-        <v>7.999593643819701E-2</v>
+        <f>1/6*(G89+2*H89+2*I89+J89)*$H$79</f>
+        <v>2.8620117192896664E-2</v>
       </c>
     </row>
     <row r="90" spans="1:11" x14ac:dyDescent="0.3">
@@ -5175,27 +5219,27 @@
       </c>
       <c r="F90" s="1">
         <f>F89+K89</f>
-        <v>1.079995936438197</v>
+        <v>1.0286201171928966</v>
       </c>
       <c r="G90" s="1">
-        <f t="shared" ref="G90:G95" si="53">($E90)*SIN($F90)^3</f>
-        <v>0.34301301710616244</v>
+        <f t="shared" ref="G90:G95" si="53">($F90)*SIN($E90)^3</f>
+        <v>0.11334921277324482</v>
       </c>
       <c r="H90" s="1">
-        <f t="shared" ref="H90:H92" si="54">($E90+0.5*$H$79)*SIN($F90+0.5*G90*$H$79)^3</f>
-        <v>0.8559064859877038</v>
+        <f t="shared" ref="H90:I90" si="54">($F90+0.5*G90*$H$87)*SIN($E90+0.5*$H$87)^3</f>
+        <v>0.33474979930856058</v>
       </c>
       <c r="I90" s="1">
-        <f t="shared" ref="I90:I92" si="55">($E90+0.5*$H$79)*SIN($F90+0.5*H90*$H$79)^3</f>
-        <v>0.99408898900670484</v>
+        <f t="shared" si="54"/>
+        <v>0.35227978691260559</v>
       </c>
       <c r="J90" s="1">
-        <f t="shared" ref="J90:J92" si="56">($E90+$H$79)*SIN($F90+I90*$H$79)^3</f>
-        <v>1.0083361425082487</v>
+        <f t="shared" ref="J90:J95" si="55">($F90+I90*$H$87)*SIN($E90+$H$87)^3</f>
+        <v>0.71782400886036013</v>
       </c>
       <c r="K90" s="22">
-        <f t="shared" ref="K90:K92" si="57">1/6*(G90+2*H90+2*I90+J90)*$H$79</f>
-        <v>0.84189001826720467</v>
+        <f t="shared" ref="K90:K92" si="56">1/6*(G90+2*H90+2*I90+J90)*$H$79</f>
+        <v>0.36753873234598955</v>
       </c>
     </row>
     <row r="91" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -5211,27 +5255,27 @@
       </c>
       <c r="F91" s="1">
         <f>F90+K90</f>
-        <v>1.9218859547054017</v>
+        <v>1.3961588495388861</v>
       </c>
       <c r="G91" s="1">
         <f t="shared" si="53"/>
-        <v>0.82793211539752065</v>
+        <v>0.83186388452736415</v>
       </c>
       <c r="H91" s="1">
-        <f t="shared" si="54"/>
-        <v>0.56301265227262143</v>
+        <f t="shared" ref="H91:I91" si="57">($F91+0.5*G91*$H$87)*SIN($E91+0.5*$H$87)^3</f>
+        <v>1.3709312612397651</v>
       </c>
       <c r="I91" s="1">
+        <f t="shared" si="57"/>
+        <v>1.4861068867781408</v>
+      </c>
+      <c r="J91" s="1">
         <f t="shared" si="55"/>
-        <v>0.78685903226879605</v>
-      </c>
-      <c r="J91" s="1">
+        <v>2.1231762642121725</v>
+      </c>
+      <c r="K91" s="22">
         <f t="shared" si="56"/>
-        <v>0.14760260167171077</v>
-      </c>
-      <c r="K91" s="22">
-        <f t="shared" si="57"/>
-        <v>0.612546347692011</v>
+        <v>1.4448527407958913</v>
       </c>
     </row>
     <row r="92" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -5240,27 +5284,27 @@
       </c>
       <c r="F92" s="1">
         <f>F91+K91</f>
-        <v>2.5344323023974127</v>
+        <v>2.8410115903347775</v>
       </c>
       <c r="G92" s="1">
         <f t="shared" si="53"/>
-        <v>0.27857629972709042</v>
+        <v>2.819714712229179</v>
       </c>
       <c r="H92" s="1">
-        <f t="shared" si="54"/>
-        <v>0.18345328177324757</v>
+        <f t="shared" ref="H92:I92" si="58">($F92+0.5*G92*$H$87)*SIN($E92+0.5*$H$87)^3</f>
+        <v>3.3782991464522212</v>
       </c>
       <c r="I92" s="1">
+        <f t="shared" si="58"/>
+        <v>3.5113432175959312</v>
+      </c>
+      <c r="J92" s="1">
         <f t="shared" si="55"/>
-        <v>0.23951838258943389</v>
-      </c>
-      <c r="J92" s="1">
+        <v>3.4559102852152614</v>
+      </c>
+      <c r="K92" s="22">
         <f t="shared" si="56"/>
-        <v>0.11607324474317993</v>
-      </c>
-      <c r="K92" s="22">
-        <f t="shared" si="57"/>
-        <v>0.20676547886593891</v>
+        <v>3.3424849542567903</v>
       </c>
     </row>
     <row r="93" spans="1:11" x14ac:dyDescent="0.3">
@@ -5277,28 +5321,28 @@
         <v>2</v>
       </c>
       <c r="F93" s="1">
-        <f t="shared" ref="F93:F95" si="58">F92+K92</f>
-        <v>2.7411977812633515</v>
+        <f t="shared" ref="F93:F95" si="59">F92+K92</f>
+        <v>6.1834965445915682</v>
       </c>
       <c r="G93" s="1">
         <f t="shared" si="53"/>
-        <v>0.11843917663418889</v>
+        <v>4.648919314491553</v>
       </c>
       <c r="H93" s="1">
-        <f t="shared" ref="H93:H95" si="59">($E93+0.5*$H$79)*SIN($F93+0.5*G93*$H$79)^3</f>
-        <v>9.3647853535401629E-2</v>
+        <f t="shared" ref="H93:I93" si="60">($F93+0.5*G93*$H$87)*SIN($E93+0.5*$H$87)^3</f>
+        <v>3.4601594465333765</v>
       </c>
       <c r="I93" s="1">
-        <f t="shared" ref="I93:I95" si="60">($E93+0.5*$H$79)*SIN($F93+0.5*H93*$H$79)^3</f>
-        <v>0.10377902627417546</v>
+        <f t="shared" si="60"/>
+        <v>3.3201699316171238</v>
       </c>
       <c r="J93" s="1">
-        <f t="shared" ref="J93:J95" si="61">($E93+$H$79)*SIN($F93+I93*$H$79)^3</f>
-        <v>7.4910575552715492E-2</v>
+        <f t="shared" si="55"/>
+        <v>1.6813039643409637</v>
       </c>
       <c r="K93" s="22">
-        <f t="shared" ref="K93:K95" si="62">1/6*(G93+2*H93+2*I93+J93)*$H$79</f>
-        <v>9.803391863434309E-2</v>
+        <f t="shared" ref="K93:K95" si="61">1/6*(G93+2*H93+2*I93+J93)*$H$79</f>
+        <v>3.3151470058555859</v>
       </c>
     </row>
     <row r="94" spans="1:11" x14ac:dyDescent="0.3">
@@ -5315,28 +5359,28 @@
         <v>2.5</v>
       </c>
       <c r="F94" s="1">
-        <f t="shared" si="58"/>
-        <v>2.8392316998976947</v>
+        <f t="shared" si="59"/>
+        <v>9.498643550447154</v>
       </c>
       <c r="G94" s="1">
         <f t="shared" si="53"/>
-        <v>6.6009160653764096E-2</v>
+        <v>2.036073321358757</v>
       </c>
       <c r="H94" s="1">
-        <f t="shared" si="59"/>
-        <v>5.6534049184353743E-2</v>
+        <f t="shared" ref="H94:I94" si="62">($F94+0.5*G94*$H$87)*SIN($E94+0.5*$H$87)^3</f>
+        <v>0.55637287469263352</v>
       </c>
       <c r="I94" s="1">
-        <f t="shared" si="60"/>
-        <v>5.9492843810290685E-2</v>
+        <f t="shared" si="62"/>
+        <v>0.53580700223904509</v>
       </c>
       <c r="J94" s="1">
+        <f t="shared" si="55"/>
+        <v>2.7447754742120755E-2</v>
+      </c>
+      <c r="K94" s="22">
         <f t="shared" si="61"/>
-        <v>4.8679469039912035E-2</v>
-      </c>
-      <c r="K94" s="22">
-        <f t="shared" si="62"/>
-        <v>5.7790402613827493E-2</v>
+        <v>0.7079801383273725</v>
       </c>
     </row>
     <row r="95" spans="1:11" x14ac:dyDescent="0.3">
@@ -5354,28 +5398,28 @@
         <v>3</v>
       </c>
       <c r="F95" s="1">
-        <f t="shared" si="58"/>
-        <v>2.8970221025115221</v>
+        <f t="shared" si="59"/>
+        <v>10.206623688774526</v>
       </c>
       <c r="G95" s="1">
         <f t="shared" si="53"/>
-        <v>4.2591127425710418E-2</v>
+        <v>2.8684539405322743E-2</v>
       </c>
       <c r="H95" s="1">
-        <f t="shared" si="59"/>
-        <v>3.7996627887763659E-2</v>
+        <f t="shared" ref="H95:I95" si="63">($F95+0.5*G95*$H$87)*SIN($E95+0.5*$H$87)^3</f>
+        <v>-1.2936307286771507E-2</v>
       </c>
       <c r="I95" s="1">
-        <f t="shared" si="60"/>
-        <v>3.9161301461512164E-2</v>
+        <f t="shared" si="63"/>
+        <v>-1.2923128539997117E-2</v>
       </c>
       <c r="J95" s="1">
+        <f t="shared" si="55"/>
+        <v>-0.44027450175576721</v>
+      </c>
+      <c r="K95" s="22">
         <f t="shared" si="61"/>
-        <v>3.3942589687427076E-2</v>
-      </c>
-      <c r="K95" s="22">
-        <f t="shared" si="62"/>
-        <v>3.8474929301948187E-2</v>
+        <v>-7.7218139000663613E-2</v>
       </c>
     </row>
     <row r="96" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -5383,7 +5427,7 @@
         <v>0.5</v>
       </c>
       <c r="B96" s="1">
-        <f>B95+C95*$C$93</f>
+        <f t="shared" ref="B96:B101" si="64">B95+C95*$C$93</f>
         <v>1</v>
       </c>
       <c r="C96" s="22">
@@ -5394,8 +5438,8 @@
         <v>80</v>
       </c>
       <c r="F96" s="26">
-        <f>ABS(F92-B91)/B91</f>
-        <v>0.33186421099960084</v>
+        <f>ABS(F95-B91)/B91</f>
+        <v>1.6907053563351451</v>
       </c>
       <c r="G96" s="11"/>
       <c r="H96" s="11"/>
@@ -5408,11 +5452,11 @@
         <v>1</v>
       </c>
       <c r="B97" s="1">
-        <f>B96+C96*$C$93</f>
+        <f t="shared" si="64"/>
         <v>1.0550977036510694</v>
       </c>
       <c r="C97" s="22">
-        <f t="shared" ref="C96:C98" si="63">B97*SIN(A97)^3</f>
+        <f t="shared" ref="C97:C98" si="65">B97*SIN(A97)^3</f>
         <v>0.62865172870906505</v>
       </c>
     </row>
@@ -5421,11 +5465,11 @@
         <v>1.5</v>
       </c>
       <c r="B98" s="1">
-        <f>B97+C97*$C$93</f>
+        <f t="shared" si="64"/>
         <v>1.3694235680056019</v>
       </c>
       <c r="C98" s="22">
-        <f t="shared" si="63"/>
+        <f t="shared" si="65"/>
         <v>1.3591580531087364</v>
       </c>
     </row>
@@ -5434,11 +5478,11 @@
         <v>2</v>
       </c>
       <c r="B99" s="1">
-        <f>B98+C98*$C$93</f>
+        <f t="shared" si="64"/>
         <v>2.0490025945599699</v>
       </c>
       <c r="C99" s="22">
-        <f t="shared" ref="C99:C101" si="64">B99*SIN(A99)^3</f>
+        <f t="shared" ref="C99:C101" si="66">B99*SIN(A99)^3</f>
         <v>1.5404953602868612</v>
       </c>
     </row>
@@ -5447,11 +5491,11 @@
         <v>2.5</v>
       </c>
       <c r="B100" s="1">
-        <f>B99+C99*$C$93</f>
+        <f t="shared" si="64"/>
         <v>2.8192502747034007</v>
       </c>
       <c r="C100" s="22">
-        <f t="shared" si="64"/>
+        <f t="shared" si="66"/>
         <v>0.60431789445206818</v>
       </c>
       <c r="E100" s="16" t="s">
@@ -5469,11 +5513,11 @@
         <v>3</v>
       </c>
       <c r="B101" s="1">
-        <f>B100+C100*$C$93</f>
+        <f t="shared" si="64"/>
         <v>3.1214092219294347</v>
       </c>
       <c r="C101" s="22">
-        <f t="shared" si="64"/>
+        <f t="shared" si="66"/>
         <v>8.7723608273171261E-3</v>
       </c>
       <c r="E101" s="6" t="s">
@@ -5481,11 +5525,11 @@
       </c>
       <c r="F101" s="27">
         <f>ABS(F95-F84)/F95</f>
-        <v>4.991362053834137E-2</v>
+        <v>0.63526679810851872</v>
       </c>
       <c r="G101" s="28">
         <f>ABS(B91-F95)/B91</f>
-        <v>0.23627703672251496</v>
+        <v>1.6907053563351451</v>
       </c>
     </row>
     <row r="102" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -5507,6 +5551,235 @@
       <c r="G102" s="30">
         <f>ABS(B91-B101)/B91</f>
         <v>0.17712333001983524</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="107" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A107" s="19" t="s">
+        <v>83</v>
+      </c>
+      <c r="B107" s="20" t="s">
+        <v>85</v>
+      </c>
+      <c r="C107" s="20">
+        <v>1</v>
+      </c>
+      <c r="D107" s="20"/>
+      <c r="E107" s="21"/>
+    </row>
+    <row r="108" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A108" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="B108" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C108" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D108" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="E108" s="31" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A109" s="9">
+        <v>0</v>
+      </c>
+      <c r="B109" s="1">
+        <v>1</v>
+      </c>
+      <c r="C109" s="1">
+        <v>2</v>
+      </c>
+      <c r="D109" s="22">
+        <f>4-0.1*B109-0.2*C109</f>
+        <v>3.5</v>
+      </c>
+      <c r="E109" s="1">
+        <f>-0.5*B109+C109*A109</f>
+        <v>-0.5</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A110" s="23">
+        <v>1</v>
+      </c>
+      <c r="B110" s="24">
+        <f>B109+E109*$C$107</f>
+        <v>0.5</v>
+      </c>
+      <c r="C110" s="24">
+        <f>C109+D109*$C$107</f>
+        <v>5.5</v>
+      </c>
+      <c r="D110" s="22">
+        <f>4-0.1*B110-0.2*C110</f>
+        <v>2.85</v>
+      </c>
+      <c r="E110" s="1">
+        <f>-0.5*B110+C110*A110</f>
+        <v>5.25</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A111" s="23">
+        <v>2</v>
+      </c>
+      <c r="B111" s="24">
+        <f>B110+E110*$C$107</f>
+        <v>5.75</v>
+      </c>
+      <c r="C111" s="24">
+        <f>C110+D110*$C$107</f>
+        <v>8.35</v>
+      </c>
+      <c r="D111" s="22">
+        <f>4-0.1*B111-0.2*C111</f>
+        <v>1.7549999999999999</v>
+      </c>
+      <c r="E111" s="1">
+        <f>-0.5*B111+C111*A111</f>
+        <v>13.824999999999999</v>
+      </c>
+    </row>
+    <row r="115" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A115" t="s">
+        <v>87</v>
+      </c>
+      <c r="C115" t="s">
+        <v>92</v>
+      </c>
+      <c r="D115">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="116" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A116" t="s">
+        <v>71</v>
+      </c>
+      <c r="B116" t="s">
+        <v>22</v>
+      </c>
+      <c r="C116" t="s">
+        <v>75</v>
+      </c>
+      <c r="D116" t="s">
+        <v>76</v>
+      </c>
+      <c r="E116" t="s">
+        <v>77</v>
+      </c>
+      <c r="F116" t="s">
+        <v>78</v>
+      </c>
+      <c r="G116" t="s">
+        <v>89</v>
+      </c>
+      <c r="H116" t="s">
+        <v>88</v>
+      </c>
+      <c r="I116" t="s">
+        <v>90</v>
+      </c>
+      <c r="J116" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="117" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A117">
+        <v>0</v>
+      </c>
+      <c r="B117">
+        <v>1</v>
+      </c>
+      <c r="C117">
+        <v>0</v>
+      </c>
+      <c r="D117">
+        <v>7.8410000000000007E-3</v>
+      </c>
+      <c r="E117">
+        <v>2.5850000000000001E-2</v>
+      </c>
+      <c r="F117">
+        <v>0.18432999999999999</v>
+      </c>
+      <c r="G117">
+        <v>0.70994000000000002</v>
+      </c>
+      <c r="H117">
+        <v>0.50707000000000002</v>
+      </c>
+      <c r="I117">
+        <f>$B$117+(37/378*$C$117+250/621*$E$117+125/594*$F$117+512/1771*$H$117)*$D$115</f>
+        <v>1.1957916390614216</v>
+      </c>
+      <c r="J117">
+        <f>$B$117+(2825/27648*$C$117+18575/48384*$E$117+13525/55296*$F$117+277/14336*G117+1/4*$H$117)*$D$115</f>
+        <v>1.1954947497364832</v>
+      </c>
+    </row>
+    <row r="118" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A118" t="s">
+        <v>94</v>
+      </c>
+      <c r="B118">
+        <f>B117+0</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="119" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A119" t="s">
+        <v>93</v>
+      </c>
+      <c r="B119">
+        <f>I117-J117</f>
+        <v>2.968893249384319E-4</v>
+      </c>
+    </row>
+    <row r="120" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A120" t="s">
+        <v>95</v>
+      </c>
+      <c r="B120" s="32">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="121" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A121" t="s">
+        <v>96</v>
+      </c>
+      <c r="B121" s="32">
+        <f>B120*B118</f>
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="122" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A122" t="s">
+        <v>97</v>
+      </c>
+      <c r="B122">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="123" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A123" t="s">
+        <v>99</v>
+      </c>
+      <c r="B123">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="124" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A124" t="s">
+        <v>98</v>
+      </c>
+      <c r="B124" s="32">
+        <f>B123*D115*ABS(B121/B119)^B122</f>
+        <v>0.60945457488459132</v>
       </c>
     </row>
   </sheetData>

</xml_diff>